<commit_message>
worldmap with context, fixed bug on countries, cleaned csv, update to country component
</commit_message>
<xml_diff>
--- a/src/data/cleaned/iso_list.xlsx
+++ b/src/data/cleaned/iso_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="742">
   <si>
     <t>country</t>
   </si>
@@ -500,9 +500,6 @@
   </si>
   <si>
     <t>COG</t>
-  </si>
-  <si>
-    <t>Democratic Republic of the Congo</t>
   </si>
   <si>
     <t>CD</t>
@@ -2619,12 +2616,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="31.290714285714284" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3220,2134 +3217,2136 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>317</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>335</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>338</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>341</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>344</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>346</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C125" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C126" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C127" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B133" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="C133" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B134" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="C134" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="C135" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B136" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="C136" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>407</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="C137" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>410</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B138" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="C138" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>413</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="C139" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>419</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="C141" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="C142" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="C143" s="2" t="s">
         <v>427</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>428</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="C145" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>434</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
       <c r="A146" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="C146" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
       <c r="A147" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>440</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
       <c r="A148" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B149" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
       <c r="A150" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B150" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
       <c r="A151" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B151" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="C151" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>452</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
       <c r="A152" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="C152" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
       <c r="A153" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="C153" s="2" t="s">
         <v>457</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>458</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B154" s="2"/>
       <c r="C154" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="C155" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
       <c r="A156" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B156" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="C156" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
       <c r="A157" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B157" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="C157" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
       <c r="A158" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B158" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="C158" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>472</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
       <c r="A159" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B159" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="C159" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
       <c r="A160" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B160" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="C160" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
       <c r="A161" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="C161" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
       <c r="A162" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="C162" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="C165" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
       <c r="A166" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="C166" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>496</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="C167" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>499</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
       <c r="A168" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="C168" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>502</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
       <c r="A169" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="C169" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>505</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
       <c r="A170" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>508</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
       <c r="A171" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="C171" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
       <c r="A172" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
       <c r="A173" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>522</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>523</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>526</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>532</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="C180" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
       <c r="A181" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>541</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
       <c r="A182" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="C182" s="2" t="s">
         <v>543</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>544</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
       <c r="A183" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="C183" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>547</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="C184" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="C185" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="C185" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="C186" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="C187" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="C188" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>562</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="C189" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>565</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="C190" s="2" t="s">
         <v>567</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>568</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="C191" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>571</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="C192" s="2" t="s">
         <v>573</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>574</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="C193" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
       <c r="A194" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="C194" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>580</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
       <c r="A195" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="C195" s="2" t="s">
         <v>582</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>583</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
       <c r="A196" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="C196" s="2" t="s">
         <v>585</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>586</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
       <c r="A197" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="C197" s="2" t="s">
         <v>588</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>589</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
       <c r="A198" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="C198" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>592</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
       <c r="A199" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="C199" s="2" t="s">
         <v>594</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>595</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
       <c r="A200" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="B200" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>597</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>598</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
       <c r="A201" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B201" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="C201" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>601</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="C202" s="2" t="s">
         <v>603</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>604</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
       <c r="A203" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B203" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="C203" s="2" t="s">
         <v>606</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>607</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
       <c r="A204" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="B204" s="2" t="s">
+      <c r="C204" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>610</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75">
       <c r="A205" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="C205" s="2" t="s">
         <v>612</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>613</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75">
       <c r="A206" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>614</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="C206" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="C206" s="2" t="s">
-        <v>616</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
       <c r="A207" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="B207" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="C207" s="2" t="s">
         <v>618</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>619</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
       <c r="A208" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="C208" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="C208" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18.75">
       <c r="A209" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="C209" s="2" t="s">
         <v>624</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>625</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
       <c r="A210" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="C210" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>628</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18.75">
       <c r="A211" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="C211" s="2" t="s">
         <v>630</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>631</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18.75">
       <c r="A212" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="B212" s="2" t="s">
+      <c r="C212" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>634</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18.75">
       <c r="A213" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="B213" s="2" t="s">
+      <c r="C213" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="C213" s="2" t="s">
-        <v>637</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18.75">
       <c r="A214" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="C214" s="2" t="s">
         <v>639</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18.75">
       <c r="A215" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="C215" s="2" t="s">
         <v>642</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>643</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18.75">
       <c r="A216" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="C216" s="2" t="s">
         <v>645</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>646</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
       <c r="A217" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="C217" s="2" t="s">
         <v>648</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>649</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="18.75">
       <c r="A218" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="C218" s="2" t="s">
         <v>651</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>652</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="18.75">
       <c r="A219" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="C219" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>655</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="18.75">
       <c r="A220" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="B220" s="2" t="s">
+      <c r="C220" s="2" t="s">
         <v>657</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>658</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="18.75">
       <c r="A221" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="B221" s="2" t="s">
+      <c r="C221" s="2" t="s">
         <v>660</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>661</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18.75">
       <c r="A222" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="B222" s="2" t="s">
+      <c r="C222" s="2" t="s">
         <v>663</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>664</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="18.75">
       <c r="A223" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="C223" s="2" t="s">
         <v>666</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>667</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="18.75">
       <c r="A224" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="C224" s="2" t="s">
         <v>669</v>
-      </c>
-      <c r="C224" s="2" t="s">
-        <v>670</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="18.75">
       <c r="A225" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="B225" s="2" t="s">
+      <c r="C225" s="2" t="s">
         <v>672</v>
-      </c>
-      <c r="C225" s="2" t="s">
-        <v>673</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="18.75">
       <c r="A226" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="B226" s="2" t="s">
+      <c r="C226" s="2" t="s">
         <v>675</v>
-      </c>
-      <c r="C226" s="2" t="s">
-        <v>676</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18.75">
       <c r="A227" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="B227" s="2" t="s">
+      <c r="C227" s="2" t="s">
         <v>678</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>679</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="18.75">
       <c r="A228" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B228" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="B228" s="2" t="s">
+      <c r="C228" s="2" t="s">
         <v>681</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>682</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18.75">
       <c r="A229" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="C229" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>685</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75">
       <c r="A230" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="B230" s="2" t="s">
+      <c r="C230" s="2" t="s">
         <v>687</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>688</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="18.75">
       <c r="A231" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="C231" s="2" t="s">
         <v>690</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>691</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75">
       <c r="A232" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="B232" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="C232" s="2" t="s">
         <v>693</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>694</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="18.75">
       <c r="A233" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="C233" s="2" t="s">
         <v>696</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>697</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75">
       <c r="A234" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="B234" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="B234" s="2" t="s">
+      <c r="C234" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>700</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="18.75">
       <c r="A235" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B235" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="C235" s="2" t="s">
         <v>702</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>703</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="18.75">
       <c r="A236" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="C236" s="2" t="s">
         <v>705</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>706</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="18.75">
       <c r="A237" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="B237" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="C237" s="2" t="s">
         <v>708</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>709</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="18.75">
       <c r="A238" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="C238" s="2" t="s">
         <v>711</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>712</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="18.75">
       <c r="A239" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="B239" s="2" t="s">
         <v>713</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="C239" s="2" t="s">
         <v>714</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>715</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75">
       <c r="A240" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="B240" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="C240" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="C240" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="18.75">
       <c r="A241" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="B241" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="C241" s="2" t="s">
         <v>720</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>721</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="18.75">
       <c r="A242" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="B242" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="C242" s="2" t="s">
         <v>723</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>724</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="18.75">
       <c r="A243" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="B243" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="B243" s="2" t="s">
+      <c r="C243" s="2" t="s">
         <v>726</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>727</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="18.75">
       <c r="A244" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="B244" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="C244" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="18.75">
       <c r="A245" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B245" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="C245" s="2" t="s">
         <v>732</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>733</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="18.75">
       <c r="A246" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B246" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="B246" s="2" t="s">
+      <c r="C246" s="2" t="s">
         <v>735</v>
-      </c>
-      <c r="C246" s="2" t="s">
-        <v>736</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="18.75">
       <c r="A247" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="B247" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="C247" s="2" t="s">
         <v>738</v>
-      </c>
-      <c r="C247" s="2" t="s">
-        <v>739</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="18.75">
       <c r="A248" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="B248" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="B248" s="2" t="s">
+      <c r="C248" s="2" t="s">
         <v>741</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>